<commit_message>
parser for mike terry data finished, writes to whatever database with URI given as argument, e.g. mongodb://127.0.0.1:3001/meteor for localhost
</commit_message>
<xml_diff>
--- a/mturk/mturk_data.xlsx
+++ b/mturk/mturk_data.xlsx
@@ -1545,22 +1545,22 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.0</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10.0</c:v>
@@ -1569,13 +1569,13 @@
                   <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>7.0</c:v>
@@ -1596,11 +1596,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="2129212248"/>
-        <c:axId val="2129219000"/>
+        <c:axId val="2073225000"/>
+        <c:axId val="2073218136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2129212248"/>
+        <c:axId val="2073225000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1629,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129219000"/>
+        <c:crossAx val="2073218136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1637,7 +1637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2129219000"/>
+        <c:axId val="2073218136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1667,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129212248"/>
+        <c:crossAx val="2073225000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2043,13 +2043,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="6" max="6" width="69.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2205,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -2248,13 +2249,13 @@
         <v>2.0833333333333333E-3</v>
       </c>
       <c r="O4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -2297,13 +2298,13 @@
         <v>2.7777777777777779E-3</v>
       </c>
       <c r="O5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -2346,13 +2347,13 @@
         <v>3.472222222222222E-3</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6">
         <v>1</v>
       </c>
       <c r="Q6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -2401,7 +2402,7 @@
         <v>1</v>
       </c>
       <c r="Q7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -2444,101 +2445,98 @@
         <v>4.8611111111111112E-3</v>
       </c>
       <c r="O8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>185</v>
+        <v>400</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>401</v>
       </c>
       <c r="G9" t="s">
-        <v>187</v>
+        <v>402</v>
       </c>
       <c r="H9" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I9" t="s">
-        <v>189</v>
+        <v>404</v>
       </c>
       <c r="J9" t="b">
         <v>1</v>
       </c>
-      <c r="K9" t="s">
-        <v>14</v>
-      </c>
       <c r="L9">
         <f>TIMEVALUE(I9)</f>
-        <v>3.2712500000000003E-3</v>
+        <v>1.0413310185185185E-3</v>
       </c>
       <c r="M9">
         <f>TIMEVALUE("0:08:00")</f>
         <v>5.5555555555555558E-3</v>
       </c>
       <c r="O9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P9">
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>190</v>
+        <v>405</v>
       </c>
       <c r="F10" t="s">
-        <v>191</v>
+        <v>406</v>
       </c>
       <c r="G10" t="s">
-        <v>192</v>
+        <v>407</v>
       </c>
       <c r="H10" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I10" t="s">
-        <v>193</v>
+        <v>408</v>
       </c>
       <c r="J10" t="s">
         <v>14</v>
       </c>
       <c r="L10">
         <f>TIMEVALUE(I10)</f>
-        <v>3.6293287037037036E-3</v>
+        <v>1.3235995370370372E-3</v>
       </c>
       <c r="M10">
         <f>TIMEVALUE("0:09:00")</f>
@@ -2556,38 +2554,38 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>194</v>
+        <v>409</v>
       </c>
       <c r="F11" t="s">
-        <v>195</v>
+        <v>410</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>411</v>
       </c>
       <c r="H11" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I11" t="s">
-        <v>197</v>
+        <v>412</v>
       </c>
       <c r="J11" t="s">
         <v>14</v>
       </c>
       <c r="L11">
         <f>TIMEVALUE(I11)</f>
-        <v>4.0989814814814821E-3</v>
+        <v>1.5604282407407407E-3</v>
       </c>
       <c r="M11">
         <f>TIMEVALUE("0:10:00")</f>
@@ -2605,143 +2603,143 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>198</v>
+        <v>413</v>
       </c>
       <c r="F12" t="s">
-        <v>199</v>
+        <v>414</v>
       </c>
       <c r="G12" t="s">
-        <v>200</v>
+        <v>415</v>
       </c>
       <c r="H12" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I12" t="s">
-        <v>201</v>
+        <v>416</v>
       </c>
       <c r="J12" t="s">
         <v>14</v>
       </c>
       <c r="L12">
         <f>TIMEVALUE(I12)</f>
-        <v>4.7317013888888886E-3</v>
+        <v>1.7386574074074075E-3</v>
       </c>
       <c r="M12">
         <f>TIMEVALUE("0:11:00")</f>
         <v>7.6388888888888886E-3</v>
       </c>
       <c r="O12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P12">
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>202</v>
+        <v>417</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
+        <v>418</v>
       </c>
       <c r="G13" t="s">
-        <v>204</v>
+        <v>419</v>
       </c>
       <c r="H13" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I13" t="s">
-        <v>205</v>
+        <v>420</v>
       </c>
       <c r="J13" t="s">
         <v>14</v>
       </c>
       <c r="L13">
         <f>TIMEVALUE(I13)</f>
-        <v>5.5608680555555559E-3</v>
+        <v>2.1090046296296295E-3</v>
       </c>
       <c r="M13">
         <f>TIMEVALUE("0:12:00")</f>
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="O13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>421</v>
       </c>
       <c r="F14" t="s">
-        <v>207</v>
+        <v>422</v>
       </c>
       <c r="G14" t="s">
-        <v>208</v>
+        <v>423</v>
       </c>
       <c r="H14" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I14" t="s">
-        <v>209</v>
+        <v>424</v>
       </c>
       <c r="J14" t="s">
         <v>14</v>
       </c>
       <c r="L14">
         <f>TIMEVALUE(I14)</f>
-        <v>7.3539351851851847E-3</v>
+        <v>2.5606828703703707E-3</v>
       </c>
       <c r="M14">
         <f>TIMEVALUE("0:13:00")</f>
         <v>9.0277777777777787E-3</v>
       </c>
       <c r="O14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P14">
         <v>1</v>
@@ -2752,38 +2750,38 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>210</v>
+        <v>425</v>
       </c>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>426</v>
       </c>
       <c r="G15" t="s">
-        <v>212</v>
+        <v>427</v>
       </c>
       <c r="H15" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I15" t="s">
-        <v>213</v>
+        <v>428</v>
       </c>
       <c r="J15" t="s">
         <v>14</v>
       </c>
       <c r="L15">
         <f>TIMEVALUE(I15)</f>
-        <v>7.75236111111111E-3</v>
+        <v>4.9799189814814819E-3</v>
       </c>
       <c r="M15">
         <f>TIMEVALUE("0:14:00")</f>
@@ -2796,43 +2794,43 @@
         <v>1</v>
       </c>
       <c r="Q15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:18">
       <c r="A16">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>184</v>
+        <v>399</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>214</v>
+        <v>429</v>
       </c>
       <c r="F16" t="s">
-        <v>215</v>
+        <v>430</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>431</v>
       </c>
       <c r="H16" t="s">
-        <v>188</v>
+        <v>403</v>
       </c>
       <c r="I16" t="s">
-        <v>217</v>
+        <v>432</v>
       </c>
       <c r="J16" t="s">
         <v>14</v>
       </c>
       <c r="L16">
         <f>TIMEVALUE(I16)</f>
-        <v>8.5373148148148153E-3</v>
+        <v>6.0443171296296295E-3</v>
       </c>
       <c r="M16">
         <f>TIMEVALUE("0:15:00")</f>
@@ -2845,43 +2843,43 @@
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>218</v>
+        <v>171</v>
       </c>
       <c r="F17" t="s">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="G17" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="H17" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="I17" t="s">
-        <v>221</v>
-      </c>
-      <c r="J17" t="s">
-        <v>14</v>
+        <v>175</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
       <c r="L17">
         <f>TIMEVALUE(I17)</f>
-        <v>9.3757870370370384E-3</v>
+        <v>5.5263657407407405E-3</v>
       </c>
       <c r="O17">
         <v>1</v>
@@ -2895,907 +2893,916 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>222</v>
+        <v>176</v>
       </c>
       <c r="F18" t="s">
-        <v>223</v>
+        <v>177</v>
       </c>
       <c r="G18" t="s">
-        <v>224</v>
+        <v>178</v>
       </c>
       <c r="H18" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="J18" t="s">
         <v>14</v>
       </c>
       <c r="L18">
         <f>TIMEVALUE(I18)</f>
-        <v>9.9925925925925928E-3</v>
+        <v>8.8131597222222222E-3</v>
       </c>
     </row>
     <row r="19" spans="1:17">
       <c r="A19">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>399</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
         <v>170</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>400</v>
+        <v>180</v>
       </c>
       <c r="F19" t="s">
-        <v>401</v>
+        <v>181</v>
       </c>
       <c r="G19" t="s">
-        <v>402</v>
+        <v>182</v>
       </c>
       <c r="H19" t="s">
-        <v>403</v>
+        <v>174</v>
       </c>
       <c r="I19" t="s">
-        <v>404</v>
-      </c>
-      <c r="J19" t="b">
-        <v>1</v>
+        <v>183</v>
+      </c>
+      <c r="J19" t="s">
+        <v>14</v>
       </c>
       <c r="L19">
         <f>TIMEVALUE(I19)</f>
-        <v>1.0413310185185185E-3</v>
+        <v>9.4679166666666679E-3</v>
       </c>
     </row>
     <row r="20" spans="1:17">
       <c r="A20">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C20" t="s">
         <v>170</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>405</v>
+        <v>390</v>
       </c>
       <c r="F20" t="s">
-        <v>406</v>
+        <v>391</v>
       </c>
       <c r="G20" t="s">
-        <v>407</v>
+        <v>392</v>
       </c>
       <c r="H20" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="I20" t="s">
-        <v>408</v>
-      </c>
-      <c r="J20" t="s">
-        <v>14</v>
+        <v>394</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>437</v>
       </c>
       <c r="L20">
         <f>TIMEVALUE(I20)</f>
-        <v>1.3235995370370372E-3</v>
+        <v>5.9584490740740743E-3</v>
       </c>
     </row>
     <row r="21" spans="1:17">
       <c r="A21">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="C21" t="s">
         <v>170</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="F21" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="G21" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="H21" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="I21" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="J21" t="s">
         <v>14</v>
+      </c>
+      <c r="K21" t="s">
+        <v>437</v>
       </c>
       <c r="L21">
         <f>TIMEVALUE(I21)</f>
-        <v>1.5604282407407407E-3</v>
+        <v>1.0544733796296295E-2</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="C22" t="s">
         <v>170</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>413</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>414</v>
+        <v>228</v>
       </c>
       <c r="G22" t="s">
-        <v>415</v>
+        <v>229</v>
       </c>
       <c r="H22" t="s">
-        <v>403</v>
+        <v>230</v>
       </c>
       <c r="I22" t="s">
-        <v>416</v>
-      </c>
-      <c r="J22" t="s">
-        <v>14</v>
+        <v>231</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
       </c>
       <c r="L22">
         <f>TIMEVALUE(I22)</f>
-        <v>1.7386574074074075E-3</v>
+        <v>1.6808564814814817E-3</v>
       </c>
     </row>
     <row r="23" spans="1:17">
       <c r="A23">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="C23" t="s">
         <v>170</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>417</v>
+        <v>232</v>
       </c>
       <c r="F23" t="s">
-        <v>418</v>
+        <v>233</v>
       </c>
       <c r="G23" t="s">
-        <v>419</v>
+        <v>234</v>
       </c>
       <c r="H23" t="s">
-        <v>403</v>
+        <v>230</v>
       </c>
       <c r="I23" t="s">
-        <v>420</v>
+        <v>235</v>
       </c>
       <c r="J23" t="s">
         <v>14</v>
       </c>
       <c r="L23">
         <f>TIMEVALUE(I23)</f>
-        <v>2.1090046296296295E-3</v>
+        <v>2.0246643518518517E-3</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s">
         <v>170</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>421</v>
+        <v>236</v>
       </c>
       <c r="F24" t="s">
-        <v>422</v>
+        <v>237</v>
       </c>
       <c r="G24" t="s">
-        <v>423</v>
+        <v>238</v>
       </c>
       <c r="H24" t="s">
-        <v>403</v>
+        <v>230</v>
       </c>
       <c r="I24" t="s">
-        <v>424</v>
+        <v>239</v>
       </c>
       <c r="J24" t="s">
         <v>14</v>
       </c>
       <c r="L24">
         <f>TIMEVALUE(I24)</f>
-        <v>2.5606828703703707E-3</v>
+        <v>3.7082523148148153E-3</v>
       </c>
     </row>
     <row r="25" spans="1:17">
       <c r="A25">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="C25" t="s">
         <v>170</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>425</v>
+        <v>240</v>
       </c>
       <c r="F25" t="s">
-        <v>426</v>
+        <v>241</v>
       </c>
       <c r="G25" t="s">
-        <v>427</v>
+        <v>242</v>
       </c>
       <c r="H25" t="s">
-        <v>403</v>
+        <v>230</v>
       </c>
       <c r="I25" t="s">
-        <v>428</v>
+        <v>243</v>
       </c>
       <c r="J25" t="s">
         <v>14</v>
       </c>
       <c r="L25">
         <f>TIMEVALUE(I25)</f>
-        <v>4.9799189814814819E-3</v>
+        <v>4.5014699074074072E-3</v>
       </c>
     </row>
     <row r="26" spans="1:17">
       <c r="A26">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="B26" t="s">
-        <v>399</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
         <v>170</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>429</v>
+        <v>244</v>
       </c>
       <c r="F26" t="s">
-        <v>430</v>
+        <v>245</v>
       </c>
       <c r="G26" t="s">
-        <v>431</v>
+        <v>246</v>
       </c>
       <c r="H26" t="s">
-        <v>403</v>
+        <v>230</v>
       </c>
       <c r="I26" t="s">
-        <v>432</v>
+        <v>247</v>
       </c>
       <c r="J26" t="s">
         <v>14</v>
       </c>
       <c r="L26">
         <f>TIMEVALUE(I26)</f>
-        <v>6.0443171296296295E-3</v>
+        <v>4.7255324074074075E-3</v>
       </c>
     </row>
     <row r="27" spans="1:17">
       <c r="A27">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D27">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>304</v>
+        <v>248</v>
       </c>
       <c r="F27" t="s">
-        <v>305</v>
+        <v>249</v>
       </c>
       <c r="G27" t="s">
-        <v>306</v>
+        <v>250</v>
       </c>
       <c r="H27" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I27" t="s">
-        <v>308</v>
-      </c>
-      <c r="J27" t="b">
-        <v>1</v>
+        <v>251</v>
+      </c>
+      <c r="J27" t="s">
+        <v>14</v>
       </c>
       <c r="L27">
         <f>TIMEVALUE(I27)</f>
-        <v>6.5490740740740743E-4</v>
+        <v>5.5390509259259256E-3</v>
       </c>
     </row>
     <row r="28" spans="1:17">
       <c r="A28">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D28">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>309</v>
+        <v>252</v>
       </c>
       <c r="F28" t="s">
-        <v>310</v>
+        <v>253</v>
       </c>
       <c r="G28" t="s">
-        <v>311</v>
+        <v>254</v>
       </c>
       <c r="H28" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I28" t="s">
-        <v>312</v>
+        <v>255</v>
       </c>
       <c r="J28" t="s">
         <v>14</v>
       </c>
       <c r="L28">
         <f>TIMEVALUE(I28)</f>
-        <v>1.0767592592592593E-3</v>
+        <v>7.0753935185185182E-3</v>
       </c>
     </row>
     <row r="29" spans="1:17">
       <c r="A29">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D29">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>313</v>
+        <v>256</v>
       </c>
       <c r="F29" t="s">
-        <v>314</v>
+        <v>257</v>
       </c>
       <c r="G29" t="s">
-        <v>315</v>
+        <v>258</v>
       </c>
       <c r="H29" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I29" t="s">
-        <v>316</v>
+        <v>259</v>
       </c>
       <c r="J29" t="s">
         <v>14</v>
       </c>
       <c r="L29">
         <f>TIMEVALUE(I29)</f>
-        <v>1.4004513888888888E-3</v>
+        <v>7.7529629629629624E-3</v>
       </c>
     </row>
     <row r="30" spans="1:17">
       <c r="A30">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D30">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>317</v>
+        <v>260</v>
       </c>
       <c r="F30" t="s">
-        <v>318</v>
+        <v>261</v>
       </c>
       <c r="G30" t="s">
-        <v>319</v>
+        <v>262</v>
       </c>
       <c r="H30" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I30" t="s">
-        <v>320</v>
+        <v>263</v>
       </c>
       <c r="J30" t="s">
         <v>14</v>
       </c>
       <c r="L30">
         <f>TIMEVALUE(I30)</f>
-        <v>1.7371180555555558E-3</v>
+        <v>7.8332870370370379E-3</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D31">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>321</v>
+        <v>264</v>
       </c>
       <c r="F31" t="s">
-        <v>322</v>
+        <v>265</v>
       </c>
       <c r="G31" t="s">
-        <v>323</v>
+        <v>266</v>
       </c>
       <c r="H31" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I31" t="s">
-        <v>324</v>
+        <v>267</v>
       </c>
       <c r="J31" t="s">
         <v>14</v>
       </c>
       <c r="L31">
         <f>TIMEVALUE(I31)</f>
-        <v>1.9973148148148146E-3</v>
+        <v>8.178287037037036E-3</v>
       </c>
     </row>
     <row r="32" spans="1:17">
       <c r="A32">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C32" t="s">
-        <v>8</v>
+        <v>170</v>
       </c>
       <c r="D32">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>325</v>
+        <v>268</v>
       </c>
       <c r="F32" t="s">
-        <v>326</v>
+        <v>269</v>
       </c>
       <c r="G32" t="s">
-        <v>327</v>
+        <v>270</v>
       </c>
       <c r="H32" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="I32" t="s">
-        <v>328</v>
+        <v>271</v>
       </c>
       <c r="J32" t="s">
         <v>14</v>
       </c>
       <c r="L32">
         <f>TIMEVALUE(I32)</f>
-        <v>2.3084606481481485E-3</v>
+        <v>9.648958333333334E-3</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C33" t="s">
         <v>8</v>
       </c>
       <c r="D33">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E33" t="s">
-        <v>337</v>
+        <v>185</v>
       </c>
       <c r="F33" t="s">
-        <v>338</v>
+        <v>186</v>
       </c>
       <c r="G33" t="s">
-        <v>339</v>
+        <v>187</v>
       </c>
       <c r="H33" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I33" t="s">
-        <v>340</v>
-      </c>
-      <c r="J33" t="s">
+        <v>189</v>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
         <v>14</v>
       </c>
       <c r="L33">
         <f>TIMEVALUE(I33)</f>
-        <v>4.1900578703703709E-3</v>
+        <v>3.2712500000000003E-3</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
         <v>8</v>
       </c>
       <c r="D34">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E34" t="s">
-        <v>345</v>
+        <v>190</v>
       </c>
       <c r="F34" t="s">
-        <v>346</v>
+        <v>191</v>
       </c>
       <c r="G34" t="s">
-        <v>347</v>
+        <v>192</v>
       </c>
       <c r="H34" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I34" t="s">
-        <v>348</v>
+        <v>193</v>
       </c>
       <c r="J34" t="s">
         <v>14</v>
       </c>
       <c r="L34">
         <f>TIMEVALUE(I34)</f>
-        <v>4.3215162037037033E-3</v>
+        <v>3.6293287037037036E-3</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C35" t="s">
         <v>8</v>
       </c>
       <c r="D35">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>349</v>
+        <v>194</v>
       </c>
       <c r="F35" t="s">
-        <v>350</v>
+        <v>195</v>
       </c>
       <c r="G35" t="s">
-        <v>351</v>
+        <v>196</v>
       </c>
       <c r="H35" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I35" t="s">
-        <v>352</v>
+        <v>197</v>
       </c>
       <c r="J35" t="s">
         <v>14</v>
       </c>
       <c r="L35">
         <f>TIMEVALUE(I35)</f>
-        <v>4.8411342592592594E-3</v>
+        <v>4.0989814814814821E-3</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="A36">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
       </c>
       <c r="D36">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>353</v>
+        <v>198</v>
       </c>
       <c r="F36" t="s">
-        <v>354</v>
+        <v>199</v>
       </c>
       <c r="G36" t="s">
-        <v>355</v>
+        <v>200</v>
       </c>
       <c r="H36" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I36" t="s">
-        <v>356</v>
+        <v>201</v>
       </c>
       <c r="J36" t="s">
         <v>14</v>
       </c>
       <c r="L36">
         <f>TIMEVALUE(I36)</f>
-        <v>5.6467013888888895E-3</v>
+        <v>4.7317013888888886E-3</v>
       </c>
     </row>
     <row r="37" spans="1:12">
       <c r="A37">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
       </c>
       <c r="D37">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E37" t="s">
-        <v>357</v>
+        <v>202</v>
       </c>
       <c r="F37" t="s">
-        <v>358</v>
+        <v>203</v>
       </c>
       <c r="G37" t="s">
-        <v>359</v>
+        <v>204</v>
       </c>
       <c r="H37" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I37" t="s">
-        <v>360</v>
+        <v>205</v>
       </c>
       <c r="J37" t="s">
         <v>14</v>
       </c>
       <c r="L37">
         <f>TIMEVALUE(I37)</f>
-        <v>5.9856597222222229E-3</v>
+        <v>5.5608680555555559E-3</v>
       </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B38" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
       </c>
       <c r="D38">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>361</v>
+        <v>206</v>
       </c>
       <c r="F38" t="s">
-        <v>362</v>
+        <v>207</v>
       </c>
       <c r="G38" t="s">
-        <v>363</v>
+        <v>208</v>
       </c>
       <c r="H38" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I38" t="s">
-        <v>364</v>
+        <v>209</v>
       </c>
       <c r="J38" t="s">
         <v>14</v>
       </c>
       <c r="L38">
         <f>TIMEVALUE(I38)</f>
-        <v>6.4304282407407418E-3</v>
+        <v>7.3539351851851847E-3</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B39" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
       </c>
       <c r="D39">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E39" t="s">
-        <v>365</v>
+        <v>210</v>
       </c>
       <c r="F39" t="s">
-        <v>366</v>
+        <v>211</v>
       </c>
       <c r="G39" t="s">
-        <v>367</v>
+        <v>212</v>
       </c>
       <c r="H39" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I39" t="s">
-        <v>368</v>
+        <v>213</v>
       </c>
       <c r="J39" t="s">
         <v>14</v>
       </c>
       <c r="L39">
         <f>TIMEVALUE(I39)</f>
-        <v>6.7057754629629637E-3</v>
+        <v>7.75236111111111E-3</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
       </c>
       <c r="D40">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E40" t="s">
-        <v>369</v>
+        <v>214</v>
       </c>
       <c r="F40" t="s">
-        <v>370</v>
+        <v>215</v>
       </c>
       <c r="G40" t="s">
-        <v>371</v>
+        <v>216</v>
       </c>
       <c r="H40" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I40" t="s">
-        <v>372</v>
+        <v>217</v>
       </c>
       <c r="J40" t="s">
         <v>14</v>
       </c>
       <c r="L40">
         <f>TIMEVALUE(I40)</f>
-        <v>7.698472222222222E-3</v>
+        <v>8.5373148148148153E-3</v>
       </c>
     </row>
     <row r="41" spans="1:12">
       <c r="A41">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
       </c>
       <c r="D41">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>373</v>
+        <v>218</v>
       </c>
       <c r="F41" t="s">
-        <v>374</v>
+        <v>219</v>
       </c>
       <c r="G41" t="s">
-        <v>375</v>
+        <v>220</v>
       </c>
       <c r="H41" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I41" t="s">
-        <v>376</v>
+        <v>221</v>
       </c>
       <c r="J41" t="s">
         <v>14</v>
       </c>
       <c r="L41">
         <f>TIMEVALUE(I41)</f>
-        <v>7.9055092592592597E-3</v>
+        <v>9.3757870370370384E-3</v>
       </c>
     </row>
     <row r="42" spans="1:12">
       <c r="A42">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>303</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
       </c>
       <c r="D42">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>377</v>
+        <v>222</v>
       </c>
       <c r="F42" t="s">
-        <v>378</v>
+        <v>223</v>
       </c>
       <c r="G42" t="s">
-        <v>379</v>
+        <v>224</v>
       </c>
       <c r="H42" t="s">
-        <v>307</v>
+        <v>188</v>
       </c>
       <c r="I42" t="s">
-        <v>380</v>
+        <v>225</v>
       </c>
       <c r="J42" t="s">
         <v>14</v>
       </c>
       <c r="L42">
         <f>TIMEVALUE(I42)</f>
-        <v>8.817662037037037E-3</v>
+        <v>9.9925925925925928E-3</v>
       </c>
     </row>
     <row r="43" spans="1:12">
       <c r="A43">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
         <v>303</v>
@@ -3807,31 +3814,31 @@
         <v>18</v>
       </c>
       <c r="E43" t="s">
-        <v>381</v>
+        <v>304</v>
       </c>
       <c r="F43" t="s">
-        <v>382</v>
+        <v>305</v>
       </c>
       <c r="G43" t="s">
-        <v>383</v>
+        <v>306</v>
       </c>
       <c r="H43" t="s">
         <v>307</v>
       </c>
       <c r="I43" t="s">
-        <v>384</v>
-      </c>
-      <c r="J43" t="s">
-        <v>14</v>
+        <v>308</v>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
       </c>
       <c r="L43">
         <f>TIMEVALUE(I43)</f>
-        <v>9.1602893518518518E-3</v>
+        <v>6.5490740740740743E-4</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="A44">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
         <v>303</v>
@@ -3843,971 +3850,965 @@
         <v>18</v>
       </c>
       <c r="E44" t="s">
-        <v>385</v>
+        <v>309</v>
       </c>
       <c r="F44" t="s">
-        <v>386</v>
+        <v>310</v>
       </c>
       <c r="G44" t="s">
-        <v>387</v>
+        <v>311</v>
       </c>
       <c r="H44" t="s">
         <v>307</v>
       </c>
       <c r="I44" t="s">
-        <v>388</v>
+        <v>312</v>
       </c>
       <c r="J44" t="s">
         <v>14</v>
       </c>
       <c r="L44">
         <f>TIMEVALUE(I44)</f>
-        <v>9.4652083333333324E-3</v>
+        <v>1.0767592592592593E-3</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="A45">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>303</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D45">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E45" t="s">
-        <v>171</v>
+        <v>313</v>
       </c>
       <c r="F45" t="s">
-        <v>172</v>
+        <v>314</v>
       </c>
       <c r="G45" t="s">
-        <v>173</v>
+        <v>315</v>
       </c>
       <c r="H45" t="s">
-        <v>174</v>
+        <v>307</v>
       </c>
       <c r="I45" t="s">
-        <v>175</v>
-      </c>
-      <c r="J45" t="b">
-        <v>1</v>
+        <v>316</v>
+      </c>
+      <c r="J45" t="s">
+        <v>14</v>
       </c>
       <c r="L45">
         <f>TIMEVALUE(I45)</f>
-        <v>5.5263657407407405E-3</v>
+        <v>1.4004513888888888E-3</v>
       </c>
     </row>
     <row r="46" spans="1:12">
       <c r="A46">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>169</v>
+        <v>303</v>
       </c>
       <c r="C46" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E46" t="s">
-        <v>176</v>
+        <v>317</v>
       </c>
       <c r="F46" t="s">
-        <v>177</v>
+        <v>318</v>
       </c>
       <c r="G46" t="s">
-        <v>178</v>
+        <v>319</v>
       </c>
       <c r="H46" t="s">
-        <v>174</v>
+        <v>307</v>
       </c>
       <c r="I46" t="s">
-        <v>179</v>
+        <v>320</v>
       </c>
       <c r="J46" t="s">
         <v>14</v>
       </c>
       <c r="L46">
         <f>TIMEVALUE(I46)</f>
-        <v>8.8131597222222222E-3</v>
+        <v>1.7371180555555558E-3</v>
       </c>
     </row>
     <row r="47" spans="1:12">
       <c r="A47">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B47" t="s">
-        <v>169</v>
+        <v>303</v>
       </c>
       <c r="C47" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D47">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E47" t="s">
-        <v>180</v>
+        <v>321</v>
       </c>
       <c r="F47" t="s">
-        <v>181</v>
+        <v>322</v>
       </c>
       <c r="G47" t="s">
-        <v>182</v>
+        <v>323</v>
       </c>
       <c r="H47" t="s">
-        <v>174</v>
+        <v>307</v>
       </c>
       <c r="I47" t="s">
-        <v>183</v>
+        <v>324</v>
       </c>
       <c r="J47" t="s">
         <v>14</v>
       </c>
       <c r="L47">
         <f>TIMEVALUE(I47)</f>
-        <v>9.4679166666666679E-3</v>
+        <v>1.9973148148148146E-3</v>
       </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E48" t="s">
-        <v>273</v>
+        <v>325</v>
       </c>
       <c r="F48" t="s">
-        <v>274</v>
+        <v>326</v>
       </c>
       <c r="G48" t="s">
-        <v>275</v>
+        <v>327</v>
       </c>
       <c r="H48" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="I48" t="s">
-        <v>277</v>
-      </c>
-      <c r="J48" t="b">
-        <v>1</v>
+        <v>328</v>
+      </c>
+      <c r="J48" t="s">
+        <v>14</v>
       </c>
       <c r="L48">
         <f>TIMEVALUE(I48)</f>
-        <v>5.2001273148148145E-3</v>
+        <v>2.3084606481481485E-3</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B49" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
       </c>
       <c r="D49">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E49" t="s">
-        <v>278</v>
+        <v>337</v>
       </c>
       <c r="F49" t="s">
-        <v>114</v>
+        <v>338</v>
       </c>
       <c r="G49" t="s">
-        <v>279</v>
+        <v>339</v>
       </c>
       <c r="H49" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="I49" t="s">
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="J49" t="s">
         <v>14</v>
-      </c>
-      <c r="K49" t="s">
-        <v>439</v>
       </c>
       <c r="L49">
         <f>TIMEVALUE(I49)</f>
-        <v>5.2448495370370366E-3</v>
+        <v>4.1900578703703709E-3</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="A50">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="D50">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E50" t="s">
-        <v>291</v>
+        <v>345</v>
       </c>
       <c r="F50" t="s">
-        <v>292</v>
+        <v>346</v>
       </c>
       <c r="G50" t="s">
-        <v>293</v>
+        <v>347</v>
       </c>
       <c r="H50" t="s">
-        <v>276</v>
+        <v>307</v>
       </c>
       <c r="I50" t="s">
-        <v>294</v>
+        <v>348</v>
       </c>
       <c r="J50" t="s">
         <v>14</v>
       </c>
       <c r="L50">
         <f>TIMEVALUE(I50)</f>
-        <v>7.8368518518518518E-3</v>
+        <v>4.3215162037037033E-3</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>389</v>
+        <v>303</v>
       </c>
       <c r="C51" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E51" t="s">
-        <v>390</v>
+        <v>349</v>
       </c>
       <c r="F51" t="s">
-        <v>391</v>
+        <v>350</v>
       </c>
       <c r="G51" t="s">
-        <v>392</v>
+        <v>351</v>
       </c>
       <c r="H51" t="s">
-        <v>393</v>
+        <v>307</v>
       </c>
       <c r="I51" t="s">
-        <v>394</v>
-      </c>
-      <c r="J51" t="b">
-        <v>1</v>
-      </c>
-      <c r="K51" t="s">
-        <v>437</v>
+        <v>352</v>
+      </c>
+      <c r="J51" t="s">
+        <v>14</v>
       </c>
       <c r="L51">
         <f>TIMEVALUE(I51)</f>
-        <v>5.9584490740740743E-3</v>
+        <v>4.8411342592592594E-3</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>389</v>
+        <v>303</v>
       </c>
       <c r="C52" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D52">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E52" t="s">
-        <v>395</v>
+        <v>353</v>
       </c>
       <c r="F52" t="s">
-        <v>396</v>
+        <v>354</v>
       </c>
       <c r="G52" t="s">
-        <v>397</v>
+        <v>355</v>
       </c>
       <c r="H52" t="s">
-        <v>393</v>
+        <v>307</v>
       </c>
       <c r="I52" t="s">
-        <v>398</v>
+        <v>356</v>
       </c>
       <c r="J52" t="s">
         <v>14</v>
-      </c>
-      <c r="K52" t="s">
-        <v>437</v>
       </c>
       <c r="L52">
         <f>TIMEVALUE(I52)</f>
-        <v>1.0544733796296295E-2</v>
+        <v>5.6467013888888895E-3</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
       </c>
       <c r="D53">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
-        <v>9</v>
+        <v>357</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>358</v>
       </c>
       <c r="G53" t="s">
-        <v>11</v>
+        <v>359</v>
       </c>
       <c r="H53" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I53" t="s">
-        <v>13</v>
-      </c>
-      <c r="J53" t="b">
-        <v>1</v>
+        <v>360</v>
+      </c>
+      <c r="J53" t="s">
+        <v>14</v>
       </c>
       <c r="L53">
         <f>TIMEVALUE(I53)</f>
-        <v>1.1315162037037036E-3</v>
+        <v>5.9856597222222229E-3</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E54" t="s">
-        <v>15</v>
+        <v>361</v>
       </c>
       <c r="F54" t="s">
-        <v>16</v>
+        <v>362</v>
       </c>
       <c r="G54" t="s">
-        <v>17</v>
+        <v>363</v>
       </c>
       <c r="H54" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I54" t="s">
-        <v>18</v>
+        <v>364</v>
       </c>
       <c r="J54" t="s">
         <v>14</v>
       </c>
       <c r="L54">
         <f>TIMEVALUE(I54)</f>
-        <v>1.6304050925925924E-3</v>
+        <v>6.4304282407407418E-3</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E55" t="s">
-        <v>19</v>
+        <v>365</v>
       </c>
       <c r="F55" t="s">
-        <v>20</v>
+        <v>366</v>
       </c>
       <c r="G55" t="s">
-        <v>21</v>
+        <v>367</v>
       </c>
       <c r="H55" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I55" t="s">
-        <v>22</v>
+        <v>368</v>
       </c>
       <c r="J55" t="s">
         <v>14</v>
       </c>
       <c r="L55">
         <f>TIMEVALUE(I55)</f>
-        <v>1.9986111111111112E-3</v>
+        <v>6.7057754629629637E-3</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E56" t="s">
-        <v>23</v>
+        <v>369</v>
       </c>
       <c r="F56" t="s">
-        <v>24</v>
+        <v>370</v>
       </c>
       <c r="G56" t="s">
-        <v>25</v>
+        <v>371</v>
       </c>
       <c r="H56" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I56" t="s">
-        <v>26</v>
+        <v>372</v>
       </c>
       <c r="J56" t="s">
         <v>14</v>
       </c>
       <c r="L56">
         <f>TIMEVALUE(I56)</f>
-        <v>3.3886111111111113E-3</v>
+        <v>7.698472222222222E-3</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>373</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>374</v>
       </c>
       <c r="G57" t="s">
-        <v>29</v>
+        <v>375</v>
       </c>
       <c r="H57" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I57" t="s">
-        <v>30</v>
+        <v>376</v>
       </c>
       <c r="J57" t="s">
         <v>14</v>
       </c>
       <c r="L57">
         <f>TIMEVALUE(I57)</f>
-        <v>5.9191435185185189E-3</v>
+        <v>7.9055092592592597E-3</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
       </c>
       <c r="D58">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E58" t="s">
-        <v>31</v>
+        <v>377</v>
       </c>
       <c r="F58" t="s">
-        <v>32</v>
+        <v>378</v>
       </c>
       <c r="G58" t="s">
-        <v>33</v>
+        <v>379</v>
       </c>
       <c r="H58" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I58" t="s">
-        <v>34</v>
+        <v>380</v>
       </c>
       <c r="J58" t="s">
         <v>14</v>
       </c>
       <c r="L58">
         <f>TIMEVALUE(I58)</f>
-        <v>7.2712268518518516E-3</v>
+        <v>8.817662037037037E-3</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
       <c r="D59">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>381</v>
       </c>
       <c r="F59" t="s">
-        <v>36</v>
+        <v>382</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
+        <v>383</v>
       </c>
       <c r="H59" t="s">
-        <v>12</v>
+        <v>307</v>
       </c>
       <c r="I59" t="s">
-        <v>38</v>
+        <v>384</v>
       </c>
       <c r="J59" t="s">
         <v>14</v>
       </c>
       <c r="L59">
         <f>TIMEVALUE(I59)</f>
-        <v>9.5883333333333324E-3</v>
+        <v>9.1602893518518518E-3</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="A60">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
-        <v>226</v>
+        <v>303</v>
       </c>
       <c r="C60" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D60">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E60" t="s">
-        <v>227</v>
+        <v>385</v>
       </c>
       <c r="F60" t="s">
-        <v>228</v>
+        <v>386</v>
       </c>
       <c r="G60" t="s">
-        <v>229</v>
+        <v>387</v>
       </c>
       <c r="H60" t="s">
-        <v>230</v>
+        <v>307</v>
       </c>
       <c r="I60" t="s">
-        <v>231</v>
-      </c>
-      <c r="J60" t="b">
-        <v>1</v>
+        <v>388</v>
+      </c>
+      <c r="J60" t="s">
+        <v>14</v>
       </c>
       <c r="L60">
         <f>TIMEVALUE(I60)</f>
-        <v>1.6808564814814817E-3</v>
+        <v>9.4652083333333324E-3</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="C61" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D61">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>232</v>
+        <v>273</v>
       </c>
       <c r="F61" t="s">
-        <v>233</v>
+        <v>274</v>
       </c>
       <c r="G61" t="s">
-        <v>234</v>
+        <v>275</v>
       </c>
       <c r="H61" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="I61" t="s">
-        <v>235</v>
-      </c>
-      <c r="J61" t="s">
-        <v>14</v>
+        <v>277</v>
+      </c>
+      <c r="J61" t="b">
+        <v>1</v>
       </c>
       <c r="L61">
         <f>TIMEVALUE(I61)</f>
-        <v>2.0246643518518517E-3</v>
+        <v>5.2001273148148145E-3</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B62" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="C62" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D62">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>278</v>
       </c>
       <c r="F62" t="s">
-        <v>237</v>
+        <v>114</v>
       </c>
       <c r="G62" t="s">
-        <v>238</v>
+        <v>279</v>
       </c>
       <c r="H62" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="I62" t="s">
-        <v>239</v>
+        <v>280</v>
       </c>
       <c r="J62" t="s">
         <v>14</v>
+      </c>
+      <c r="K62" t="s">
+        <v>439</v>
       </c>
       <c r="L62">
         <f>TIMEVALUE(I62)</f>
-        <v>3.7082523148148153E-3</v>
+        <v>5.2448495370370366E-3</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B63" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="C63" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D63">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>240</v>
+        <v>291</v>
       </c>
       <c r="F63" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="G63" t="s">
-        <v>242</v>
+        <v>293</v>
       </c>
       <c r="H63" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="I63" t="s">
-        <v>243</v>
+        <v>294</v>
       </c>
       <c r="J63" t="s">
         <v>14</v>
       </c>
       <c r="L63">
         <f>TIMEVALUE(I63)</f>
-        <v>4.5014699074074072E-3</v>
+        <v>7.8368518518518518E-3</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D64">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" t="s">
         <v>11</v>
       </c>
-      <c r="E64" t="s">
-        <v>244</v>
-      </c>
-      <c r="F64" t="s">
-        <v>245</v>
-      </c>
-      <c r="G64" t="s">
-        <v>246</v>
-      </c>
       <c r="H64" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I64" t="s">
-        <v>247</v>
-      </c>
-      <c r="J64" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="J64" t="b">
+        <v>1</v>
       </c>
       <c r="L64">
         <f>TIMEVALUE(I64)</f>
-        <v>4.7255324074074075E-3</v>
+        <v>1.1315162037037036E-3</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="A65">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D65">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>248</v>
+        <v>15</v>
       </c>
       <c r="F65" t="s">
-        <v>249</v>
+        <v>16</v>
       </c>
       <c r="G65" t="s">
-        <v>250</v>
+        <v>17</v>
       </c>
       <c r="H65" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I65" t="s">
-        <v>251</v>
+        <v>18</v>
       </c>
       <c r="J65" t="s">
         <v>14</v>
       </c>
       <c r="L65">
         <f>TIMEVALUE(I65)</f>
-        <v>5.5390509259259256E-3</v>
+        <v>1.6304050925925924E-3</v>
       </c>
     </row>
     <row r="66" spans="1:12">
       <c r="A66">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D66">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>252</v>
+        <v>19</v>
       </c>
       <c r="F66" t="s">
-        <v>253</v>
+        <v>20</v>
       </c>
       <c r="G66" t="s">
-        <v>254</v>
+        <v>21</v>
       </c>
       <c r="H66" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I66" t="s">
-        <v>255</v>
+        <v>22</v>
       </c>
       <c r="J66" t="s">
         <v>14</v>
       </c>
       <c r="L66">
         <f>TIMEVALUE(I66)</f>
-        <v>7.0753935185185182E-3</v>
+        <v>1.9986111111111112E-3</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="A67">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B67" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D67">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>256</v>
+        <v>23</v>
       </c>
       <c r="F67" t="s">
-        <v>257</v>
+        <v>24</v>
       </c>
       <c r="G67" t="s">
-        <v>258</v>
+        <v>25</v>
       </c>
       <c r="H67" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I67" t="s">
-        <v>259</v>
+        <v>26</v>
       </c>
       <c r="J67" t="s">
         <v>14</v>
       </c>
       <c r="L67">
         <f>TIMEVALUE(I67)</f>
-        <v>7.7529629629629624E-3</v>
+        <v>3.3886111111111113E-3</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="A68">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>260</v>
+        <v>27</v>
       </c>
       <c r="F68" t="s">
-        <v>261</v>
+        <v>28</v>
       </c>
       <c r="G68" t="s">
-        <v>262</v>
+        <v>29</v>
       </c>
       <c r="H68" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I68" t="s">
-        <v>263</v>
+        <v>30</v>
       </c>
       <c r="J68" t="s">
         <v>14</v>
       </c>
       <c r="L68">
         <f>TIMEVALUE(I68)</f>
-        <v>7.8332870370370379E-3</v>
+        <v>5.9191435185185189E-3</v>
       </c>
     </row>
     <row r="69" spans="1:12">
       <c r="A69">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B69" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D69">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>264</v>
+        <v>31</v>
       </c>
       <c r="F69" t="s">
-        <v>265</v>
+        <v>32</v>
       </c>
       <c r="G69" t="s">
-        <v>266</v>
+        <v>33</v>
       </c>
       <c r="H69" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I69" t="s">
-        <v>267</v>
+        <v>34</v>
       </c>
       <c r="J69" t="s">
         <v>14</v>
       </c>
       <c r="L69">
         <f>TIMEVALUE(I69)</f>
-        <v>8.178287037037036E-3</v>
+        <v>7.2712268518518516E-3</v>
       </c>
     </row>
     <row r="70" spans="1:12">
       <c r="A70">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B70" t="s">
-        <v>226</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>170</v>
+        <v>8</v>
       </c>
       <c r="D70">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>268</v>
+        <v>35</v>
       </c>
       <c r="F70" t="s">
-        <v>269</v>
+        <v>36</v>
       </c>
       <c r="G70" t="s">
-        <v>270</v>
+        <v>37</v>
       </c>
       <c r="H70" t="s">
-        <v>230</v>
+        <v>12</v>
       </c>
       <c r="I70" t="s">
-        <v>271</v>
+        <v>38</v>
       </c>
       <c r="J70" t="s">
         <v>14</v>
       </c>
       <c r="L70">
         <f>TIMEVALUE(I70)</f>
-        <v>9.648958333333334E-3</v>
+        <v>9.5883333333333324E-3</v>
       </c>
     </row>
     <row r="71" spans="1:12">
@@ -5967,7 +5968,7 @@
         <v>440</v>
       </c>
       <c r="L102" t="e">
-        <f t="shared" ref="L66:L102" si="0">TIMEVALUE(I102)</f>
+        <f>TIMEVALUE(I102)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -5984,8 +5985,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L101">
-    <sortCondition ref="A2:A101"/>
+  <sortState ref="A2:L102">
+    <sortCondition ref="C2:C102"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>